<commit_message>
Updated price to $1.25
</commit_message>
<xml_diff>
--- a/Encodings.xlsx
+++ b/Encodings.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ricwi\Box\19S\EE 4325\Project 1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{4C311431-1D82-497C-8431-9177EBE217C8}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21158091-0B0B-40CB-ADD3-6B820D79A8C1}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="16860" windowHeight="7485" xr2:uid="{2E2DF944-95A1-4910-98B0-451B57FFCF13}"/>
   </bookViews>
@@ -409,10 +409,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{07F24E7C-686A-4E79-A557-272CCB071474}">
-  <dimension ref="A1:E8"/>
+  <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q16" sqref="Q16"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -499,8 +499,8 @@
       <c r="A7">
         <v>4</v>
       </c>
-      <c r="B7" t="s">
-        <v>5</v>
+      <c r="B7" s="1">
+        <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.45">
@@ -509,6 +509,14 @@
       </c>
       <c r="B8" t="s">
         <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A9">
+        <v>6</v>
+      </c>
+      <c r="B9" t="s">
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>